<commit_message>
Updated on 01-16-2024 at 23:06
</commit_message>
<xml_diff>
--- a/output/measles_latex.xlsx
+++ b/output/measles_latex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,9 @@
       <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -457,6 +460,9 @@
       <c r="D2" t="n">
         <v>478</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.000413</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -471,6 +477,9 @@
       <c r="D3" t="n">
         <v>7351</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.002545</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -485,6 +494,9 @@
       <c r="D4" t="n">
         <v>5227</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.00228</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -499,6 +511,9 @@
       <c r="D5" t="n">
         <v>1801</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.000651</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -513,6 +528,9 @@
       <c r="D6" t="n">
         <v>879</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.000169</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -527,6 +545,9 @@
       <c r="D7" t="n">
         <v>1013</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.000142</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -541,6 +562,9 @@
       <c r="D8" t="n">
         <v>1286</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.000111</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -555,6 +579,9 @@
       <c r="D9" t="n">
         <v>1347</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.000128</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -569,6 +596,9 @@
       <c r="D10" t="n">
         <v>1485</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.000109</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -583,6 +613,9 @@
       <c r="D11" t="n">
         <v>1566</v>
       </c>
+      <c r="E11" t="n">
+        <v>8.4e-05</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -596,6 +629,9 @@
       </c>
       <c r="D12" t="n">
         <v>623</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.000107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 01-17-2024 at 22:45
</commit_message>
<xml_diff>
--- a/output/measles_latex.xlsx
+++ b/output/measles_latex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,16 +452,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3101</v>
+        <v>0.4467</v>
       </c>
       <c r="C2" t="n">
-        <v>95</v>
+        <v>717</v>
       </c>
       <c r="D2" t="n">
-        <v>478</v>
+        <v>3895</v>
       </c>
       <c r="E2" t="n">
-        <v>0.000413</v>
+        <v>0.002557</v>
       </c>
     </row>
     <row r="3">
@@ -469,16 +469,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2455</v>
+        <v>0.4212</v>
       </c>
       <c r="C3" t="n">
-        <v>717</v>
+        <v>656</v>
       </c>
       <c r="D3" t="n">
-        <v>7351</v>
+        <v>5227</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002545</v>
+        <v>0.002309</v>
       </c>
     </row>
     <row r="4">
@@ -486,16 +486,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1758</v>
+        <v>0.388</v>
       </c>
       <c r="C4" t="n">
-        <v>656</v>
+        <v>183</v>
       </c>
       <c r="D4" t="n">
-        <v>5227</v>
+        <v>1801</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00228</v>
+        <v>0.00065</v>
       </c>
     </row>
     <row r="5">
@@ -503,16 +503,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.09995999999999999</v>
+        <v>0.02486</v>
       </c>
       <c r="C5" t="n">
-        <v>183</v>
+        <v>44</v>
       </c>
       <c r="D5" t="n">
-        <v>1801</v>
+        <v>879</v>
       </c>
       <c r="E5" t="n">
-        <v>0.000651</v>
+        <v>0.000172</v>
       </c>
     </row>
     <row r="6">
@@ -520,16 +520,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0161</v>
+        <v>0.02535</v>
       </c>
       <c r="C6" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D6" t="n">
-        <v>879</v>
+        <v>1013</v>
       </c>
       <c r="E6" t="n">
-        <v>0.000169</v>
+        <v>0.000142</v>
       </c>
     </row>
     <row r="7">
@@ -537,16 +537,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.009974</v>
+        <v>0.00942</v>
       </c>
       <c r="C7" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>1013</v>
+        <v>1286</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000142</v>
+        <v>0.000109</v>
       </c>
     </row>
     <row r="8">
@@ -554,16 +554,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.006508</v>
+        <v>0.007609</v>
       </c>
       <c r="C8" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D8" t="n">
-        <v>1286</v>
+        <v>1347</v>
       </c>
       <c r="E8" t="n">
-        <v>0.000111</v>
+        <v>0.000127</v>
       </c>
     </row>
     <row r="9">
@@ -571,16 +571,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.003821</v>
+        <v>0.003633</v>
       </c>
       <c r="C9" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" t="n">
-        <v>1347</v>
+        <v>1485</v>
       </c>
       <c r="E9" t="n">
-        <v>0.000128</v>
+        <v>0.000108</v>
       </c>
     </row>
     <row r="10">
@@ -588,16 +588,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.003156</v>
+        <v>0.003071</v>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D10" t="n">
-        <v>1485</v>
+        <v>1566</v>
       </c>
       <c r="E10" t="n">
-        <v>0.000109</v>
+        <v>8.3e-05</v>
       </c>
     </row>
     <row r="11">
@@ -605,33 +605,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.00264</v>
+        <v>0.002616</v>
       </c>
       <c r="C11" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D11" t="n">
-        <v>1566</v>
+        <v>623</v>
       </c>
       <c r="E11" t="n">
-        <v>8.4e-05</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.002055</v>
-      </c>
-      <c r="C12" t="n">
-        <v>28</v>
-      </c>
-      <c r="D12" t="n">
-        <v>623</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.000107</v>
+        <v>0.000106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>